<commit_message>
Week ending 10-18 hours
</commit_message>
<xml_diff>
--- a/BLU_ET_2020_Employees_wPTO.xlsx
+++ b/BLU_ET_2020_Employees_wPTO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://belcan-my.sharepoint.com/personal/jtreptow_belcan_com/Documents/BlueOrigin/2020_Base2_Personel/ConsultantTimeReport/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{0EAF4CD2-EB15-4C7B-9258-0D55C340C4D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3CD0FBF9-BE32-4155-BD75-85A274E740C7}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="114_{CE60D106-7C2D-4E24-ADD1-6D924F399E82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{47B827C2-8E2D-4A99-993A-B7E926B9A35A}"/>
   <bookViews>
-    <workbookView xWindow="1210" yWindow="1460" windowWidth="31050" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="1130" windowWidth="34160" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BLU_ET_2020_Employees_wPTO" sheetId="1" r:id="rId1"/>
@@ -1211,7 +1211,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AN1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AQ10" sqref="AQ10"/>
+      <selection pane="topRight" activeCell="BF35" sqref="BF35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>